<commit_message>
Bao cao ngay mai 10/5
</commit_message>
<xml_diff>
--- a/Data/Data_DemoPredicted.xlsx
+++ b/Data/Data_DemoPredicted.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,7 +384,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E mới mua con s10 được gần 2 tuần mà sao xài nhanh nóng quá ạ Hay do cài đặt e chỉnh sai gì ạ</t>
+          <t>Đèn pin có vấn đề,dc đổi cái mới nhưng cũng vậy, cảm ứng chậm, màn hình tắt đèn pin cũng tắt. Chụp hình buổi tối đèn flash lúc có lúc ko. Chắc trả hàng lại.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -399,7 +399,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Máy hết pin nhanh quá, có cách nào khắc phục không, mọi thứ đều ổn chỉ có pin là tệ, 4sao</t>
+          <t>Sản phẩm rất tốt, khả năng tự phục hồi tốt nhưng phải tìm hiểu kỹ ứng dụng mặc định của máy, nghe nhạc chất lượng hay lên theo thời gian nghe nhạc và chụp hình cũng thế, loa ngoài nghe chất lượng cao nhưng hơi rè là do loa còn mới chưa nghe nhiều nên màng loa chưa giãn nở và chưa cập nhật âm nhạc nhưng hơi gây khó ngủ nên samsung cần cải thiện vì gây ảnh hưởng cho nhiều người sử dụng, nói chung chất lượng tốt.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -414,12 +414,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dùng chưa đầy một tháng nhưng quá nhiều thất vọng thỉnh thoảng đọc báo treo không vuốt được, cảm ứng có cuộc gọi ko vuốt nghe được kém hơn cả huawei nếu ai có ý định rước em này nên suy nghĩ pin xuống nhanh nữa thất vọng</t>
+          <t>mới vừa mua một a10 xanh cho mama, đem về ai cũng thích với bề ngoài đẹp, loa ko có vấn đề, camera rõ nét, thiếu cái tai phone với ốp lưng nhân viên tuyệt vời mở hộp thấy bị trầy tự đổi cái mới cho mình lun :D</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -429,7 +429,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Màn hình cứ tự bật sáng khi bỏ túi,y như máy đểu ngày xưa, pin yếu,vân tay lì.. Quá thất vọng</t>
+          <t>Mọi thứ đều ổn. Riêng camera bị nhoè và không sắc nét, không bằng samsung j2pro 2018.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -444,12 +444,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Máy đẹp, mượt, tất cả đều hài lòng nhưng điểm yếu pin tụt quá nhanh dù tắt hết ứng dụng ngầm nên cho 4 sao</t>
+          <t>Thiết kế hơi tồi nhất là chiếc loa ngoài, màn hình nhạt sam sung tối ưu hơi kém,cấu hình ổn,mượt mà. Cùng tầm giá 3 củ mua tàu dừa ngon hơn nhiều</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Negative</t>
+          <t>Positive</t>
         </is>
       </c>
     </row>
@@ -459,7 +459,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Máy đẹp, dùng mượt, pin hơi yếu tí. Dán màn nên vân tay hơi chậm. Nói chung đến thời điểm hiện tại khá hài lòng</t>
+          <t>Đth dùng tốt, thiết kế đẹp, chỉ có cái đèn pin hay nhấp nháy khi tắt màn hình, camera đẹp không nhòe như mấy bạn khác nói, pin trâu, sạc khá nhanh.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -474,7 +474,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Máy đẹp, nhanh , ngon, chỉ tiếc là Pin tụt hơi nhanh. Còn lại mọi cái đều tuyệt vời.</t>
+          <t>Mình mới mua máy hôm qua. Theo cảm nhận của mình thì máy sài tốt. Bắt sóng wifi, 3g, 4g đều tốt cả không hề yếu như comment đánh giá của một số bạn. Loa to rõ ràng. Camera chụp hình rõ và đẹp. Có một điểm mình chưa hài lòng ở đây chính là xem video youtube toàn màn hình thì không được nét lắm thôi. Còn lại tất cả đều ổn tốt so với tầm giá 3tr. Một điểm thu hút mình ngay cái nhìn đầu tiên đó chính là vẻ ngoài của máy và màn hình giọt nước đẹp và thu hút người nhìn. Tóm lại máy tốt và nhân viên thân thiện vui vẻ.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Đã mua và sử dụng từ đời s8.rất đẹp và ok.màu xanh khá đẹp.s10 nhỏ vừa tay hơn s10+.mình đã chọn s10.</t>
+          <t>Thiết kế đẹp mới dùng vẫn cho 5* .pin dùng khá ổn máy chạy mát, hàng sam màn hình nhìn vẫn nịnh mắt ko như mấy a khựa.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -504,7 +504,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Dùng màn hình đẹp, pin hơi yếu so với dòng A, wifile bắt khoảng cách xa yếu hơn dòng lumia</t>
+          <t>Máy mới mua về xài ngon, hôm nay 6/5 tự nhiên thông báo cập nhật bảo mật gì đó của ss, cập nhật xong chẳng thấy gì, chỉ thấy bắt cài 1 số ứng dụng tào lao, mà sau cập nhật máy siêu nặng, lag chậm, chắc mai đem ra tgdđ trả hàng.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -519,12 +519,852 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Nhận máy s10 từ hôm qua tại cửa hàng ở số 3 Quang Trung, Nha Trang. Điện thoại dùng quá ngon, màu xanh của máy đẹp, màn hình sáng, pin khá ổn, chụp hình ấn tượng. Chỉ có cái cảm ứng siêu âm khi ko có dán màn hình thì quá ngon, hy vọng sớm ra dán màn hình tích hợp. Nhân viên TGDĐ nhiệt tình, cảm ơn đã giao máy đúng hẹn.</t>
+          <t>Máy dùng rất tuyệt . Chơi game nặng k vấn đề luôn . Pin rất ok . Camera nét căng đét . Nói chung miên chê ạ .</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
           <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Mua được 10 ngày. Máy sài tốt pin cực trâu. Dùng lướt web xem phim liên tục đc khoảng 10 tiếng. Tầm giá này là quá ngon rồi</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Ko còn j để nói quá tệ í lộn tuyệt vời.Nhân viên nhiệt tình.pin trâu chơi game quá ngon tầm này cho tàu khựa ế luôn</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Mới mua dc 1 tuần Máy galaxy A10 dung tốt voi giá 3tr la ổn , chơi game liên quân vs free fire đều ổn , bắt wifi tốt , pin thi choi cung ổn n, noi chung la voi mức gia 3tr ma dùng dc nhu thế la ok , mấy bạn đoi camera chup hinh nay nọ thi mua máy với muc giá cao hon di , tiền ít đòi hít đồ ngon</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mới mua ngày hôm qua máy màu đỏ, e rất thích màu đỏ, loa lớn, sóng wf và sóng dt bình thường k yếu như mọi người nói, có đèn flash thông báo nữa. Chỉ có là đèn pin mở r khi tắt màn hình là bị nháy, mở màn hình sáng lên mới có đèn pin, mọi thứ còn lại đc so với giá 3tr, pin k dực nhều (chắc tuỳ máy), 3tr như vậy là ổn r</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Máy em loa thì quá tệ bị sai màu hết bắt sống 4g yếu Tôi mún đổi tgdd nói là máy khong lỗi nhưng nó quá tệ a10</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Mới mua được hai ngày, máy xài ổn,pin trâu, chơi liên quân mượt bắt, wifi mạnh,3tr ổn</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Xài được 2tuan máy êm,bin xài cả ngày mới hết ,chụp hình rõ, so với giá 3tr quá ok</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Vừa mua hôm qua, Muốn trả lại, quá tệ. Samsung galaxy a 10 , camera quá kém, wifi quá yếu , hình ảnh khi đọc báo nhòe nhoẹt.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Mua sản phẩm A10 đc đúng 1 tuần, dùng tốt, pin ổn, chụp hình ok, chơi game k bị lag, nói chung máy ngon trong tầm 3tr. Nhân viên hỗ trợ nhiệt tình &lt;3</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sản phẩm tốt pin dùng cơ bản thì khoảng 2 ngày chơi game liên quân 1h20p hụt 17% pin nhưng có điều coi điện thoại samsung a10 rất hay bị mỏi mắt còn nhận dạng khuân mặt nhậy wf bắt cũng khỏe nói chung mua đồ điện tử tuy cùng 1 máy nhưng cũng hên xui hên mua dk máy ngon xui thì gặp máy dở chứ k phải máy nào cũng như nhau</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Giá ok, Cấu hình quá ok trong tầm giá 3tr. Bộ nhớ lớn, thiết kế đẹp. Mua cho bố mẹ, bố mẹ rất ưng. Ủng hộ dài dài</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>chơi game ổn. mua để chơi game thì ok! mượt. exynos 7884 thật ra là 7885 dùng trên mấy con cận cao cấp nhưng mà bị giảm xung nhịp còn 1.6 vẫn giữ 8 luồng xử lí cho máy giá rẻ bớt bá thôi =)). gpu maliG71mp2 thì dạng ổn rồi ko phải dạng vừa :)) ram 2gb đủ sài (đag chơi game nặng mà ng ta nhắn mesenger hay có cuộc gọi tới mà ko bị diss ra là ok rồi). Nói chung cấu hình chiến tốt game. Còn về tổng thể (thiết kế, cam, loa, pin,...) thì hơi dở, mua khuyến mãi có 2tr7 thôi nên hk dám bốc phốt nhiều hahaah.</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Mình mua máy 27/4.máy dùng rất ok.chơi lq mượt.thấy bắt wifi và camera k tệ như các bạn khác cmt.ncl trong tầm giá rất ổn.</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Sản phẩm rất tệ.Màn hình hiển thị xấu. Lúc mua không để ý về phát hiện cái loa nằm sau lưng máy úp xuống là ai gọi không nghe được chuông. Nghe nhạc xem phim thì phải luôn cầm máy vì úp xuống không nghe. Một thiết kế ngu kinh khủng</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Mua ngày 26_4 . Giá 3.090.000 .Sạc chưa đầy 5p thì nóng củ sạc . Lắp 2 sym 1 viettel 1 vina mà sóng yếu kinh khủng .</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Mọi thứ đều ổn, trừ camera hơi kém. So với mức giá trên dưới 3 triệu chất lượng như vậy là tốt rồi. Nhân viên bán hàng chu đáo.</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Samsung a10 quá tệ. Bắt sóng wifi yếu, nhận diện khuôn mặt quá tệ. Sài còn dở hơn điện thoại Trung Quốc và quá ít chức năng</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>máy tầm 3tr mà ảo quá choi game 1 tiếng mất hơn 50% ping kiểm tra thì ko thấy hao nhân viên kiểm tra vẩn vậy phải gủi trạm bảo hành</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Pin 3400 Ma sài mau hết quá đi còn lại cũng tạm được đúng là là tiền nào của đó .vậy ma nói pin sài cả ngày E sài 3/4la het</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Mới mua 20/4 xài được 6 ngay mà pin mau hết wa sắc đây pin mà xài được mấy tiếng hết rồi.pin đó wa.chỉ có pin là ko được thời còn mới thư điều tốt.</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Sài máy quá chán! Camera chụp quá tệ. Điện thoại thiết kế ra cho trẻ em thì phải? Cài đặt gmail cho google mà có 2 chế độ người lớn và trẻ em. Mà nếu lỡ ai cài phải trẻ em là nó hạn chế mọi mặt luôn. Sp quá tệ lần đầu sài ss mà thế này thì quá thất vọng</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Mới mua nên chưa đánh giá đc nhiều nhưng dùng thấy nóng, chụp ảnh chất lượng kém. Nv tại tgdd nhiệt tình.</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Mở khóa bằng khuôn mặt không được nhạy cho lắm... Còn lại là rất ok so với tầm giá 3Tr</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Mới mua hôm 22/4 h bị hư màng hình rồi kém quá ko ổn tí nào cần tìm hiểu kỉ trước khi dùng SP này</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Pin tốt lâu heêt pin.cảm ứng nhạy. riêng camera trước chụp hơi bị nhòe.nhân viên tư vấn nhiệt tình</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Mik mới mua hồi trưa nay tại dmx 288 cai nước-ca mau đầu tiên chị tư vấn Như Ý rất nhiệt tình và thân thiện dễ thương. Về máy thì rất ok pin trâu ngon , camera tạm được ,cảm ứng vô cùng nhạy. Nói chung là trên cả tuyệt vời so với tầm giá</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Với tầm giá này là ok rồi. Chơi game cũng ổn Có phần chụp ảnh thì hơi mờ. Cải thiện được thì ok</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Mới mua con này, mọi thứ đều ổn chỉ mỗi cái camera 13MP mà chụp ảnh quá tệ, không ngờ anh Sam nay lại xuống cấp như vậy, dần bị mất niềm tin vô anh Sam luôn</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Giá 3tr mà cầm em này ngon lành...chip exynos quá đỉnh...liên quân max cấu hình...lag là khi mạng yếu...ngoài ra đều tuyệt vời....tui troll ông quản lý...lấy cái xanh, xong đổi cái đỏ rồi lấy cái đen...ổng cười nhẹ....cái này là ok chưa má....hjhj nhiệt tình vui vẻ...ok very good</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Ít khi dùng camera nhưng không ngờ nó tệ đến v, không dám selfi hay chụp hình luôn. Bạn nào lâu lâu có chụp hình cũng nên né chiếc này ra</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Sản phẩm tốt với giá, nhân viên tư vấn nhiệt tình, có điều camera không được ưg ý cho lắm</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Mới mua online trên mạng độc quyền của tgdd máy khá đẹp và gọn đặc biệt màn hình 6,2 inch giọt nước và bộ nhớ trong 32g</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>mới mua 2 ngày tại tgdd bảo lâm, máy đẹp chạy mượt. nhân viên tgdd rất nhiệt tình, vui vẻ.</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Mua 2tr450 ngày 20 Nói chung ok mọi thứ pin trâu chơi liên quân FPS 31 Hình ảnh ok</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Mới nhận ĐT chiều hôm qua máy đẹp màu đỏ em rất thích... Nhân viên phục vụ nhiệt tình dù em đặt nhầm địa chỉ vẫn phục vụ rất tốt.... Cám ơn chị Hiền Thu ngân đã tư vấn nhiệt tình lần sau sẽ kô đặt nhầm địa chỉ nữa ĐT 131 PHÙNG HƯNG cám ơn anh chị nhân viên rất nhiều ạ... 😊</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Đã mua và trải nghiệm, máy sang chảnh so với giá, tất cả điều ngon, chơi liên quân mượt nếu chỉnh cấu hình thấp, mọi thứ điều ok ngoại trừ chưa đâu bán cường lực và op lưng, ko biết tắt cái game tools khi chơi game cái này hình như để cho youtuber thì ổn hơn, có chạm tắt màn hình, ko có chạm sáng màn hình, sạc từ 20 đến 95% tốn 1h40 phút, pin trâu chơi liên quân 5h và các ứng dụng khác rất lâu khoảng 8h, ko nói quá, mình có chụp hình để chứng minh bên dưới, mình ngạc nhiên về giá so với chất lượng máy nhưng ko có tai nghe, cây lấy sim thì thấy gớm như cọng kẽm, khay đựng sim hơi mỏng gồm nhựa và kim loại. Nv tgdđ rất thân thiện.</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Mới mua hôm 21.4 gần 2,8 triệu ,máy quá tuyệt vời so với giá ,nhân viên theo bến cát rất nhiệt tình. Rất hài lòng.</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Thật sự thất vọng,đt mới mua về hình ảnh và chữ bị nhòe toàn bộ..này do lỗi máy.chắc lý do đó nên kg có trưng bày ra cho khách trải nghiệm</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Mới mua hôm 21.4 gần 2,8 triệu ,máy quá tuyệt vời so với giá ,nhân viên theo bến cát rất nhiệt tình. Rất hài lòng.</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Ok chơi game pubg mượt hơn oppo A83 3gram ko có hd, A10 chơi hd ok tốt trong tầm giá cho samsung 5sao</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Máy chạy rất ok xem phim chạy mượt mà bin xài rất lâu kết wifi mạnh loa rat lớn nhiêu ung dung tu samsung Choi game khoi nói nhé kết nối không dây smart switch tiện dụng chi cần dang nhập tk cua bạn k mất thứ gì Nhưng máy k có tai nghe 😃</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Máy hợp lý giá tiền Nhu cầu xem fim, nghe gọi, fb, zalo Ram 2gb bộ nhớ 32gb đủ dùng, pin trâu 1 ngày sử dụng, đặt trước nên được giảm 300+250k khách hàng thân thiện . Mua máy có 2540k Nhân viên tạo tgdd số 342 tứ kì hải dương thân thiện phục vụ nhiệt tình</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Trong tầm giá thì máy sử dụng cũng bình thường.mới lấy hôm qua nên cũng không đánh giá được nhiều.</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Máy mới được nhận hôm 20/04. Mấy chị nhân viên ở bên TGDĐ Lãnh Binh Thăng quận 11 HCM dễ thương, tư vấn nhiệt tình. Mua để tặng ngày của mẹ nên tắt nguồn đến 3 tuần sau mới test máy được.. 😘😍</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Máy ổn, nhưng cấu hình ko đc đẹp mắt. Thiết kế phần sau máy cũng ko đc đẹp. Chụp hình đẹp</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Ko lên mua chơi geam theo mình mua Redmi mà chiến ngọt giá lại rẻ cho ae nào chơi liên quân pubg</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Máy ngon chơi game mượt giao diện đẹp pubg mức trung bình ko lag tóm lại mảy chơi game khá ngon xứng đáng đồng tiền</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Tôi có ghé ĐMX và TGDĐ ở Tân định, Bến Cát, BD. Thái độ của nhân viên ở đây không nhiệt tình lắm khi tôi hỏi mua trả góp điện thoại tầm hơn 3 triệu. Trả góp thì đã sao, đâu phải cướp bóc gì đâu tỏ vẻ coi thường. Thất vọng.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Sản phẩm rất tệ, hay đơ, loa sau đặt ở 1 vị trí chẳng thể hiểu nổi, màn hình nhìn rất rẻ tiền, tệ hơn rất nhiều so với những thương hiệu Trung Quốc, âm thanh loa trong và ngoài đều nhỏ và rè. Nhân viên dán màn hình và mặt sau quá ẩu. Thái độ thiếu tôn trọng khách hàng. Rất thất vọng, sẽ không bao giờ quay lại.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Tạm được chỉ 2790k thì ko thể đòi hỏi hơn nếu loa nằm cạnh bên thì mặt lưng đẹp hơn</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Máy rất đẹp với giá tiền 2.790.000 thì rất hài lòng . Chỉ có một điều hơi thất vọng là Pin . Bởi vì để ở chế độ chờ , sau khi đã đóng hoàn toàn các ứng dụng chạy ngầm mà sau 24 giờ Pin tuột mất tới 20% .</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Cho hỏi khi sạc thấy củ sạc rất nóng đấy có phải vấn đề.ko . Còn dùng rất mượt .................</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Máy tốt, mới mua thì hơi lag chắc là do mới khởi động, về sau thì rất mượt. Máy ảnh chụp không được đẹp nhưng dù sao vẫn tốt!</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Nói chung là được trong tầm giá nhưng nhân viê hỗ trợ kỹ thuật chưa rành lắm chắc do máy mới về còn về chụp hình thì ko dám chụp</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Điện thoại nói chung mượt và nhiều thứ tốt nhưng thiếu óp lưng và tay nghe mình chỉ đánh giá vậy thôi 5 *</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Máy hơi đơ tí nhưng nói chung là ổn rất tốt và chơi PUPG, Liên Quân hay giật tí nhưng với giá vậy là ok r</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Negative</t>
         </is>
       </c>
     </row>

</xml_diff>